<commit_message>
more scripts for analysis 2stim data
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/04-watchSSVEP-SNR/watchFftDataset.xlsx
+++ b/dataAnalysisCodes/watchERP/04-watchSSVEP-SNR/watchFftDataset.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="61">
   <si>
     <t>date</t>
   </si>
@@ -166,6 +166,39 @@
   </si>
   <si>
     <t>2013-04-10-17-27-49</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>2013-06-03-anderson</t>
+  </si>
+  <si>
+    <t>2013-06-03-14-44-02</t>
+  </si>
+  <si>
+    <t>2013-06-03-14-51-37</t>
+  </si>
+  <si>
+    <t>2013-06-03-14-59-20</t>
+  </si>
+  <si>
+    <t>2013-06-03-15-05-14</t>
+  </si>
+  <si>
+    <t>2013-06-03-15-11-19</t>
+  </si>
+  <si>
+    <t>2013-06-03-15-17-38</t>
+  </si>
+  <si>
+    <t>2013-06-03-15-23-51</t>
+  </si>
+  <si>
+    <t>2013-06-03-15-29-39</t>
   </si>
 </sst>
 </file>
@@ -521,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:D25"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,9 +565,9 @@
     <col min="1" max="1" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
@@ -1187,6 +1220,214 @@
         <v>10</v>
       </c>
       <c r="H25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="3">
+        <v>41339</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="2">
+        <v>12</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="3">
+        <v>41339</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="2">
+        <v>12</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="3">
+        <v>41339</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="2">
+        <v>10</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="3">
+        <v>41339</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="2">
+        <v>15</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="3">
+        <v>41339</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="2">
+        <v>15</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="3">
+        <v>41339</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="2">
+        <v>10</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="3">
+        <v>41339</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="3">
+        <v>41339</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H33" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
it's been a while
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/04-watchSSVEP-SNR/watchFftDataset.xlsx
+++ b/dataAnalysisCodes/watchERP/04-watchSSVEP-SNR/watchFftDataset.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="72">
   <si>
     <t>date</t>
   </si>
@@ -199,6 +199,39 @@
   </si>
   <si>
     <t>2013-06-03-15-29-39</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>Marijn</t>
+  </si>
+  <si>
+    <t>2013-06-06-marijn</t>
+  </si>
+  <si>
+    <t>2013-06-06-15-10-23</t>
+  </si>
+  <si>
+    <t>2013-06-06-15-18-33</t>
+  </si>
+  <si>
+    <t>2013-06-06-15-24-10</t>
+  </si>
+  <si>
+    <t>2013-06-06-15-29-56</t>
+  </si>
+  <si>
+    <t>2013-06-06-15-47-50</t>
+  </si>
+  <si>
+    <t>2013-06-06-15-53-20</t>
+  </si>
+  <si>
+    <t>2013-06-06-15-58-51</t>
+  </si>
+  <si>
+    <t>2013-06-06-16-04-46</t>
   </si>
 </sst>
 </file>
@@ -554,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="A35" sqref="A35:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,6 +1462,214 @@
       </c>
       <c r="H33" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="3">
+        <v>41431</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="2">
+        <v>15</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="3">
+        <v>41431</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" s="2">
+        <v>10</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="3">
+        <v>41431</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="2">
+        <v>12</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="3">
+        <v>41431</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="2">
+        <v>10</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="3">
+        <v>41431</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="2">
+        <v>15</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="3">
+        <v>41431</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" s="2">
+        <v>12</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="3">
+        <v>41431</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="3">
+        <v>41431</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back on the road
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/04-watchSSVEP-SNR/watchFftDataset.xlsx
+++ b/dataAnalysisCodes/watchERP/04-watchSSVEP-SNR/watchFftDataset.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="107">
   <si>
     <t>date</t>
   </si>
@@ -232,6 +232,111 @@
   </si>
   <si>
     <t>2013-06-06-16-04-46</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>Yelena</t>
+  </si>
+  <si>
+    <t>18/7/2013</t>
+  </si>
+  <si>
+    <t>2013-07-18-yelena</t>
+  </si>
+  <si>
+    <t>2013-07-18-15-11-12</t>
+  </si>
+  <si>
+    <t>2013-07-18-15-18-53</t>
+  </si>
+  <si>
+    <t>2013-07-18-15-26-03</t>
+  </si>
+  <si>
+    <t>2013-07-18-15-32-16</t>
+  </si>
+  <si>
+    <t>2013-07-18-15-43-31</t>
+  </si>
+  <si>
+    <t>2013-07-18-15-51-54</t>
+  </si>
+  <si>
+    <t>2013-07-18-15-58-42</t>
+  </si>
+  <si>
+    <t>2013-07-18-16-05-13</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>30/7/2013</t>
+  </si>
+  <si>
+    <t>2013-07-30-robert</t>
+  </si>
+  <si>
+    <t>2013-07-30-14-33-23</t>
+  </si>
+  <si>
+    <t>2013-07-30-14-41-12</t>
+  </si>
+  <si>
+    <t>2013-07-30-15-01-18</t>
+  </si>
+  <si>
+    <t>2013-07-30-15-08-27</t>
+  </si>
+  <si>
+    <t>2013-07-30-15-20-51</t>
+  </si>
+  <si>
+    <t>2013-07-30-15-28-11</t>
+  </si>
+  <si>
+    <t>2013-07-30-15-40-15</t>
+  </si>
+  <si>
+    <t>2013-07-30-15-47-39</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>2013-08-07-10-48-11</t>
+  </si>
+  <si>
+    <t>2013-08-07-10-58-05</t>
+  </si>
+  <si>
+    <t>2013-08-07-11-04-37</t>
+  </si>
+  <si>
+    <t>2013-08-07-11-11-34</t>
+  </si>
+  <si>
+    <t>2013-08-07-11-26-57</t>
+  </si>
+  <si>
+    <t>2013-08-07-11-33-46</t>
+  </si>
+  <si>
+    <t>2013-08-07-11-40-19</t>
+  </si>
+  <si>
+    <t>2013-08-07-11-47-18</t>
+  </si>
+  <si>
+    <t>2013-08-07-alejandro</t>
   </si>
 </sst>
 </file>
@@ -587,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:D41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,6 +1774,630 @@
         <v>8.57</v>
       </c>
       <c r="H41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="2">
+        <v>15</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="2">
+        <v>10</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G45" s="2">
+        <v>10</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G46" s="2">
+        <v>12</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="2">
+        <v>15</v>
+      </c>
+      <c r="H47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="2">
+        <v>12</v>
+      </c>
+      <c r="H49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="2">
+        <v>15</v>
+      </c>
+      <c r="H50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="2">
+        <v>15</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G52" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="2">
+        <v>12</v>
+      </c>
+      <c r="H53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55" s="2">
+        <v>10</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56" s="2">
+        <v>10</v>
+      </c>
+      <c r="H56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G57" s="2">
+        <v>12</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="3">
+        <v>41463</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G58" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="3">
+        <v>41463</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G59" s="2">
+        <v>15</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="3">
+        <v>41463</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G60" s="2">
+        <v>12</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" s="3">
+        <v>41463</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="2">
+        <v>15</v>
+      </c>
+      <c r="H61" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="3">
+        <v>41463</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62" s="2">
+        <v>12</v>
+      </c>
+      <c r="H62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" s="3">
+        <v>41463</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G63" s="2">
+        <v>8.57</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64" s="3">
+        <v>41463</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" s="2">
+        <v>10</v>
+      </c>
+      <c r="H64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C65" s="3">
+        <v>41463</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G65" s="2">
+        <v>10</v>
+      </c>
+      <c r="H65" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>